<commit_message>
03 S04 Working with variables etc
</commit_message>
<xml_diff>
--- a/excel-vba-files/introduction_to_vba/referencing_cells_sheets_books.xlsx
+++ b/excel-vba-files/introduction_to_vba/referencing_cells_sheets_books.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <workbookPr codeName="Sellest_töövihikust" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositories\VBA course\excel-vba-files\introduction_to_vba\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses" sheetId="1" r:id="rId1"/>
@@ -32,11 +37,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +59,13 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -99,17 +111,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaallaad" xfId="0" builtinId="0"/>
+    <cellStyle name="Valuuta" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -117,12 +130,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office'i kujundus">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -164,7 +180,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,9 +213,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,6 +265,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -407,7 +457,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Leht1"/>
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -416,7 +467,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="15.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
@@ -427,39 +480,39 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="3"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" s="3"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="3"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" s="3"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" s="3"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" s="3"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
+      <c r="C10" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -470,7 +523,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Leht2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>